<commit_message>
Added logs & Not Data driven but not working need to check
</commit_message>
<xml_diff>
--- a/TestData/UserData.xlsx
+++ b/TestData/UserData.xlsx
@@ -8,35 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/74692fe9ac76fb33/Desktop/API/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33FB18B1-7456-4BE2-B1DF-CD26AC7D7286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:801_{60FB8094-F1DE-48D0-86CF-BE3AE4C3DCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{308D1497-FDDB-4516-AD9C-471A514DEA52}"/>
   <bookViews>
-    <workbookView xWindow="3552" yWindow="6408" windowWidth="17280" windowHeight="8880" xr2:uid="{46EDCC07-4225-4BEE-B1D4-E751937FB872}"/>
+    <workbookView xWindow="3552" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{46EDCC07-4225-4BEE-B1D4-E751937FB872}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>UserID</t>
   </si>
@@ -96,6 +85,15 @@
   </si>
   <si>
     <t>54q</t>
+  </si>
+  <si>
+    <t>1010345</t>
+  </si>
+  <si>
+    <t>10225</t>
+  </si>
+  <si>
+    <t>1030885</t>
   </si>
 </sst>
 </file>
@@ -140,9 +138,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -461,7 +460,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,31 +471,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1010</v>
+      <c r="A2" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -518,8 +517,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1020</v>
+      <c r="A3" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -541,8 +540,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1030</v>
+      <c r="A4" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>

</xml_diff>